<commit_message>
Tried histograms, open-close next
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6600" windowWidth="28660" windowHeight="9460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28660" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Evaluation of processes on photos</t>
   </si>
@@ -82,13 +83,70 @@
   </si>
   <si>
     <t>t_noEdge_imadj</t>
+  </si>
+  <si>
+    <t>u_noEdge_imadj</t>
+  </si>
+  <si>
+    <t>2_noEdge_hist</t>
+  </si>
+  <si>
+    <t>3_noEdge_hist</t>
+  </si>
+  <si>
+    <t>11_noEdge_hist</t>
+  </si>
+  <si>
+    <t>12_noEdge_hist</t>
+  </si>
+  <si>
+    <t>e_noEdge_hist</t>
+  </si>
+  <si>
+    <t>f_noEdge_hist</t>
+  </si>
+  <si>
+    <t>g_noEdge_hist</t>
+  </si>
+  <si>
+    <t>gg_noEdge_hist</t>
+  </si>
+  <si>
+    <t>k_noEdge_hist</t>
+  </si>
+  <si>
+    <t>t_noEdge_hist</t>
+  </si>
+  <si>
+    <t>u_noEdge_hist</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
+    <t>can remove white spots??</t>
+  </si>
+  <si>
+    <t>Same as 12</t>
+  </si>
+  <si>
+    <t>nothing really</t>
+  </si>
+  <si>
+    <t>no_edge_imadj</t>
+  </si>
+  <si>
+    <t>_noEdge_hist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +158,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,14 +196,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,95 +549,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1">
+    <row r="2" spans="1:4">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -557,17 +681,211 @@
       <c r="C12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Man with a plan
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7980" windowWidth="28660" windowHeight="8300" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="840" yWindow="8720" windowWidth="25600" windowHeight="7380" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Evaluation of processes on photos</t>
   </si>
@@ -164,22 +164,40 @@
     <t>Try repeated OCing to solidify one fat line</t>
   </si>
   <si>
-    <t>axes1</t>
-  </si>
-  <si>
-    <t>panel10</t>
-  </si>
-  <si>
-    <t>panel20</t>
-  </si>
-  <si>
-    <t>panel8</t>
-  </si>
-  <si>
-    <t>panel21</t>
-  </si>
-  <si>
-    <t>panel9</t>
+    <t>Final plan:</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>hist</t>
+  </si>
+  <si>
+    <t>OC50</t>
+  </si>
+  <si>
+    <t>edge (what kind?)</t>
+  </si>
+  <si>
+    <t>D10E15</t>
+  </si>
+  <si>
+    <t>can tune</t>
+  </si>
+  <si>
+    <t>leave only largest body</t>
+  </si>
+  <si>
+    <t>fill with random points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find circle </t>
+  </si>
+  <si>
+    <t>estimate circle size</t>
   </si>
 </sst>
 </file>
@@ -192,6 +210,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,8 +255,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -252,15 +275,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,7 +620,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -962,49 +989,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E5"/>
+  <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1</v>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="C5">
-        <v>2</v>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="F4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Good progress, index error in mod rn??
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>Evaluation of processes on photos</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>estimate circle size</t>
+  </si>
+  <si>
+    <t>http://blogs.mathworks.com/pick/2008/03/14/fitting-a-circle-easily/</t>
   </si>
 </sst>
 </file>
@@ -992,7 +995,7 @@
   <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1037,6 +1040,9 @@
     <row r="4" spans="1:10">
       <c r="F4" t="s">
         <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>